<commit_message>
Yearly and Monthly Reports generation
</commit_message>
<xml_diff>
--- a/public/excel/PPE_Report.xlsx
+++ b/public/excel/PPE_Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>INVENTORY OF EQUIPMENT</t>
   </si>
@@ -26,10 +26,10 @@
     <t>For which</t>
   </si>
   <si>
-    <t>Sheila Marilie Lueilwitz</t>
-  </si>
-  <si>
-    <t>James L. Gordon Avenue Market and Mall</t>
+    <t>Boris Ida Stoltenberg</t>
+  </si>
+  <si>
+    <t>City Accounting Department</t>
   </si>
   <si>
     <t>Olongapo City is accountable having assumed such acountability on</t>
@@ -119,28 +119,61 @@
     <t>DEPRECIATION</t>
   </si>
   <si>
+    <t>Land (201) Code 1</t>
+  </si>
+  <si>
+    <t>01.51</t>
+  </si>
+  <si>
+    <t>Chart holder</t>
+  </si>
+  <si>
+    <t>Sticky Notes</t>
+  </si>
+  <si>
+    <t>2019-03-26</t>
+  </si>
+  <si>
+    <t>Bailey, Joannie</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>01.54</t>
+  </si>
+  <si>
+    <t>Emergency light</t>
+  </si>
+  <si>
+    <t>Water Dispenser</t>
+  </si>
+  <si>
+    <t>2019-04-02</t>
+  </si>
+  <si>
     <t>Office Buildings (211) Code 2</t>
   </si>
   <si>
-    <t>02.51</t>
-  </si>
-  <si>
-    <t>Chart holder</t>
-  </si>
-  <si>
-    <t>2019-12-09</t>
-  </si>
-  <si>
-    <t>Anderson, Elisabeth</t>
-  </si>
-  <si>
-    <t>Balay</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>02.510</t>
+  </si>
+  <si>
+    <t>Ball Pen</t>
+  </si>
+  <si>
+    <t>Hospitals and Health Centers (213) Code 4</t>
+  </si>
+  <si>
+    <t>04.42</t>
+  </si>
+  <si>
+    <t>Instructional Material</t>
+  </si>
+  <si>
+    <t>Water bottles</t>
   </si>
 </sst>
 </file>
@@ -551,7 +584,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A8" sqref="A8:O9"/>
@@ -559,17 +592,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="51.130371" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="71.696777" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="35.2771" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="45.845947" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="77.695313" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="23.422852" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="4.570313" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="15.281982" bestFit="true" customWidth="true" style="0"/>
@@ -711,32 +744,32 @@
       <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="C11">
-        <v>4555</v>
+      <c r="C11" t="s">
+        <v>37</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s">
         <v>39</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
       <c r="H11" t="s">
         <v>40</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>500.0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>500.0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>250000.0</v>
       </c>
       <c r="L11" t="s">
         <v>41</v>
@@ -745,45 +778,42 @@
         <v>41</v>
       </c>
       <c r="N11">
-        <v>0.9</v>
+        <v>450.0</v>
       </c>
       <c r="O11">
-        <v>0.1</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12">
-        <v>4555</v>
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" t="s">
         <v>39</v>
       </c>
       <c r="H12" t="s">
         <v>40</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>3.0</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>3.0</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>9.0</v>
       </c>
       <c r="L12" t="s">
         <v>41</v>
@@ -792,57 +822,111 @@
         <v>41</v>
       </c>
       <c r="N12">
-        <v>0.9</v>
+        <v>0.675</v>
       </c>
       <c r="O12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C13">
-        <v>4555</v>
-      </c>
-      <c r="D13">
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
         <v>40</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="I14">
+        <v>200.0</v>
+      </c>
+      <c r="J14">
+        <v>200.0</v>
+      </c>
+      <c r="K14">
+        <v>40000.0</v>
+      </c>
+      <c r="L14" t="s">
         <v>41</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M14" t="s">
         <v>41</v>
       </c>
-      <c r="N13">
-        <v>0.9</v>
-      </c>
-      <c r="O13">
-        <v>0.1</v>
+      <c r="N14">
+        <v>180.0</v>
+      </c>
+      <c r="O14">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16">
+        <v>69.0</v>
+      </c>
+      <c r="J16">
+        <v>69.0</v>
+      </c>
+      <c r="K16">
+        <v>4761.0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16">
+        <v>31.05</v>
+      </c>
+      <c r="O16">
+        <v>6.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>